<commit_message>
ideaal last varend en leeg
</commit_message>
<xml_diff>
--- a/experimenten Thijn/ideaal last.xlsx
+++ b/experimenten Thijn/ideaal last.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/tlievaart_tudelft_nl/Documents/Q4/Integratie project 1/IP-26/experimenten Thijn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:40000_{7D56AA38-1070-41F3-A451-630BC9F9711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="10_ncr:40000_{7D56AA38-1070-41F3-A451-630BC9F9711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18253128-4DFB-4D31-9F16-8CC20B183945}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="105">
   <si>
     <t>LOADING CONDITION</t>
   </si>
@@ -348,12 +350,15 @@
   </si>
   <si>
     <t xml:space="preserve"> in script</t>
+  </si>
+  <si>
+    <t>Deck is 17016 mm from WL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -699,10 +704,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection sqref="A1:A163"/>
     </sheetView>
   </sheetViews>
@@ -2668,4 +2673,3880 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6B3937-7E1D-4C75-B443-E24399BADABE}">
+  <dimension ref="A2:M163"/>
+  <sheetViews>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection sqref="A1:A163"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>39.968000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>24.984000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>178.43899999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>187.958</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>-8.9220000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>115.986</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>48.206000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>170.84200000000001</v>
+      </c>
+      <c r="C18">
+        <v>-9.9920000000000009</v>
+      </c>
+      <c r="D18">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>56693.084999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>180431.23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>79.319999999999993</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>4.0279999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>79.679000000000002</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>12.577</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24">
+        <v>0.99560000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25">
+        <v>0.94520000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>7231.134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28">
+        <v>79.638999999999996</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29">
+        <v>936333.58600000001</v>
+      </c>
+      <c r="C29" s="1">
+        <v>19826000</v>
+      </c>
+      <c r="D29" s="1">
+        <v>20762000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30">
+        <v>10315.251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34">
+        <v>29290.59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35">
+        <v>155.828</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>12.824</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36">
+        <v>140.61000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38">
+        <v>1222.229</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39">
+        <v>156.45099999999999</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>24.984000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40">
+        <v>135263.198</v>
+      </c>
+      <c r="C40">
+        <v>114119.77899999999</v>
+      </c>
+      <c r="D40">
+        <v>249382.97700000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>-11.068</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>-2.117</v>
+      </c>
+      <c r="B45">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6.8330000000000002</v>
+      </c>
+      <c r="B46">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>15.784000000000001</v>
+      </c>
+      <c r="B47">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>24.734000000000002</v>
+      </c>
+      <c r="B48">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>33.683999999999997</v>
+      </c>
+      <c r="B49">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>42.634999999999998</v>
+      </c>
+      <c r="B50">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51.585000000000001</v>
+      </c>
+      <c r="B51">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>60.534999999999997</v>
+      </c>
+      <c r="B52">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>69.486000000000004</v>
+      </c>
+      <c r="B53">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>78.436000000000007</v>
+      </c>
+      <c r="B54">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>87.387</v>
+      </c>
+      <c r="B55">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>96.337000000000003</v>
+      </c>
+      <c r="B56">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>105.28700000000001</v>
+      </c>
+      <c r="B57">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>114.238</v>
+      </c>
+      <c r="B58">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>123.188</v>
+      </c>
+      <c r="B59">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>132.13800000000001</v>
+      </c>
+      <c r="B60">
+        <v>319.03399999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>141.089</v>
+      </c>
+      <c r="B61">
+        <v>318.91500000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>150.03899999999999</v>
+      </c>
+      <c r="B62">
+        <v>318.07799999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>158.99</v>
+      </c>
+      <c r="B63">
+        <v>304.20600000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>167.94</v>
+      </c>
+      <c r="B64">
+        <v>172.535</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>176.89</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>-11.39</v>
+      </c>
+      <c r="B69">
+        <v>576.31700000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>-2.3420000000000001</v>
+      </c>
+      <c r="B70">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>6.7050000000000001</v>
+      </c>
+      <c r="B71">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>15.753</v>
+      </c>
+      <c r="B72">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>24.800999999999998</v>
+      </c>
+      <c r="B73">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>33.847999999999999</v>
+      </c>
+      <c r="B74">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>42.896000000000001</v>
+      </c>
+      <c r="B75">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>51.944000000000003</v>
+      </c>
+      <c r="B76">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>60.991</v>
+      </c>
+      <c r="B77">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>70.039000000000001</v>
+      </c>
+      <c r="B78">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>79.085999999999999</v>
+      </c>
+      <c r="B79">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>88.134</v>
+      </c>
+      <c r="B80">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>97.182000000000002</v>
+      </c>
+      <c r="B81">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>106.229</v>
+      </c>
+      <c r="B82">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>115.277</v>
+      </c>
+      <c r="B83">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>124.325</v>
+      </c>
+      <c r="B84">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>133.37200000000001</v>
+      </c>
+      <c r="B85">
+        <v>998.48500000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>142.41999999999999</v>
+      </c>
+      <c r="B86">
+        <v>998.255</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>151.46700000000001</v>
+      </c>
+      <c r="B87">
+        <v>996.81399999999996</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>160.51499999999999</v>
+      </c>
+      <c r="B88">
+        <v>942.23599999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>169.56299999999999</v>
+      </c>
+      <c r="B89">
+        <v>553.51300000000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>178.61</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>55</v>
+      </c>
+      <c r="B92">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>56</v>
+      </c>
+      <c r="B93" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>140.61000000000001</v>
+      </c>
+      <c r="B94">
+        <v>998.34400000000005</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>150.11000000000001</v>
+      </c>
+      <c r="B95">
+        <v>997.23299999999995</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>159.61000000000001</v>
+      </c>
+      <c r="B96">
+        <v>961.22900000000004</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>169.11</v>
+      </c>
+      <c r="B97">
+        <v>577.35</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>178.61</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>58</v>
+      </c>
+      <c r="B100">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>55</v>
+      </c>
+      <c r="B101">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>59</v>
+      </c>
+      <c r="B102" t="s">
+        <v>60</v>
+      </c>
+      <c r="C102" t="s">
+        <v>61</v>
+      </c>
+      <c r="D102" t="s">
+        <v>62</v>
+      </c>
+      <c r="E102" t="s">
+        <v>63</v>
+      </c>
+      <c r="F102" t="s">
+        <v>64</v>
+      </c>
+      <c r="G102" t="s">
+        <v>65</v>
+      </c>
+      <c r="H102" t="s">
+        <v>66</v>
+      </c>
+      <c r="I102" t="s">
+        <v>67</v>
+      </c>
+      <c r="J102" t="s">
+        <v>68</v>
+      </c>
+      <c r="K102" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>-11.39</v>
+      </c>
+      <c r="B103">
+        <v>102.407</v>
+      </c>
+      <c r="C103">
+        <v>1.64</v>
+      </c>
+      <c r="D103">
+        <v>-11.39</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>17.713000000000001</v>
+      </c>
+      <c r="G103">
+        <v>374.00200000000001</v>
+      </c>
+      <c r="H103">
+        <v>78.775000000000006</v>
+      </c>
+      <c r="I103">
+        <v>295.22699999999998</v>
+      </c>
+      <c r="J103">
+        <v>9.157</v>
+      </c>
+      <c r="K103">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>-2.3420000000000001</v>
+      </c>
+      <c r="B104">
+        <v>129.56</v>
+      </c>
+      <c r="C104">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D104">
+        <v>-2.3420000000000001</v>
+      </c>
+      <c r="E104">
+        <v>1E-3</v>
+      </c>
+      <c r="F104">
+        <v>12.526</v>
+      </c>
+      <c r="G104">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H104">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I104">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J104">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K104">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>6.7050000000000001</v>
+      </c>
+      <c r="B105">
+        <v>129.56</v>
+      </c>
+      <c r="C105">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D105">
+        <v>6.7050000000000001</v>
+      </c>
+      <c r="E105">
+        <v>1E-3</v>
+      </c>
+      <c r="F105">
+        <v>12.526</v>
+      </c>
+      <c r="G105">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H105">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I105">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J105">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K105">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>15.753</v>
+      </c>
+      <c r="B106">
+        <v>129.56</v>
+      </c>
+      <c r="C106">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D106">
+        <v>15.753</v>
+      </c>
+      <c r="E106">
+        <v>1E-3</v>
+      </c>
+      <c r="F106">
+        <v>12.526</v>
+      </c>
+      <c r="G106">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H106">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I106">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J106">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K106">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>24.800999999999998</v>
+      </c>
+      <c r="B107">
+        <v>129.56</v>
+      </c>
+      <c r="C107">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D107">
+        <v>24.800999999999998</v>
+      </c>
+      <c r="E107">
+        <v>1E-3</v>
+      </c>
+      <c r="F107">
+        <v>12.526</v>
+      </c>
+      <c r="G107">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H107">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I107">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J107">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K107">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>33.847999999999999</v>
+      </c>
+      <c r="B108">
+        <v>129.56</v>
+      </c>
+      <c r="C108">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D108">
+        <v>33.847999999999999</v>
+      </c>
+      <c r="E108">
+        <v>1E-3</v>
+      </c>
+      <c r="F108">
+        <v>12.526</v>
+      </c>
+      <c r="G108">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H108">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I108">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J108">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K108">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>42.896000000000001</v>
+      </c>
+      <c r="B109">
+        <v>129.56</v>
+      </c>
+      <c r="C109">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D109">
+        <v>42.896000000000001</v>
+      </c>
+      <c r="E109">
+        <v>1E-3</v>
+      </c>
+      <c r="F109">
+        <v>12.526</v>
+      </c>
+      <c r="G109">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H109">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I109">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J109">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K109">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>51.944000000000003</v>
+      </c>
+      <c r="B110">
+        <v>129.56</v>
+      </c>
+      <c r="C110">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D110">
+        <v>51.944000000000003</v>
+      </c>
+      <c r="E110">
+        <v>1E-3</v>
+      </c>
+      <c r="F110">
+        <v>12.526</v>
+      </c>
+      <c r="G110">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H110">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I110">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J110">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K110">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>60.991</v>
+      </c>
+      <c r="B111">
+        <v>129.56</v>
+      </c>
+      <c r="C111">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D111">
+        <v>60.991</v>
+      </c>
+      <c r="E111">
+        <v>1E-3</v>
+      </c>
+      <c r="F111">
+        <v>12.526</v>
+      </c>
+      <c r="G111">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H111">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I111">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J111">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K111">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>70.039000000000001</v>
+      </c>
+      <c r="B112">
+        <v>129.56</v>
+      </c>
+      <c r="C112">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D112">
+        <v>70.039000000000001</v>
+      </c>
+      <c r="E112">
+        <v>1E-3</v>
+      </c>
+      <c r="F112">
+        <v>12.526</v>
+      </c>
+      <c r="G112">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H112">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I112">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J112">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K112">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>79.085999999999999</v>
+      </c>
+      <c r="B113">
+        <v>129.56</v>
+      </c>
+      <c r="C113">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D113">
+        <v>79.085999999999999</v>
+      </c>
+      <c r="E113">
+        <v>1E-3</v>
+      </c>
+      <c r="F113">
+        <v>12.526</v>
+      </c>
+      <c r="G113">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H113">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I113">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J113">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K113">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>88.134</v>
+      </c>
+      <c r="B114">
+        <v>129.56</v>
+      </c>
+      <c r="C114">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D114">
+        <v>88.134</v>
+      </c>
+      <c r="E114">
+        <v>1E-3</v>
+      </c>
+      <c r="F114">
+        <v>12.526</v>
+      </c>
+      <c r="G114">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H114">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I114">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J114">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K114">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>97.182000000000002</v>
+      </c>
+      <c r="B115">
+        <v>129.56</v>
+      </c>
+      <c r="C115">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D115">
+        <v>97.182000000000002</v>
+      </c>
+      <c r="E115">
+        <v>1E-3</v>
+      </c>
+      <c r="F115">
+        <v>12.526</v>
+      </c>
+      <c r="G115">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H115">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I115">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J115">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K115">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>106.229</v>
+      </c>
+      <c r="B116">
+        <v>129.56</v>
+      </c>
+      <c r="C116">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D116">
+        <v>106.229</v>
+      </c>
+      <c r="E116">
+        <v>1E-3</v>
+      </c>
+      <c r="F116">
+        <v>12.526</v>
+      </c>
+      <c r="G116">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H116">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I116">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J116">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K116">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>115.277</v>
+      </c>
+      <c r="B117">
+        <v>129.56</v>
+      </c>
+      <c r="C117">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D117">
+        <v>115.277</v>
+      </c>
+      <c r="E117">
+        <v>1E-3</v>
+      </c>
+      <c r="F117">
+        <v>12.526</v>
+      </c>
+      <c r="G117">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H117">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I117">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J117">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K117">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>124.325</v>
+      </c>
+      <c r="B118">
+        <v>129.56</v>
+      </c>
+      <c r="C118">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D118">
+        <v>124.325</v>
+      </c>
+      <c r="E118">
+        <v>1E-3</v>
+      </c>
+      <c r="F118">
+        <v>12.526</v>
+      </c>
+      <c r="G118">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H118">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I118">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J118">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K118">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>133.37200000000001</v>
+      </c>
+      <c r="B119">
+        <v>129.55600000000001</v>
+      </c>
+      <c r="C119">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D119">
+        <v>133.37200000000001</v>
+      </c>
+      <c r="E119">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F119">
+        <v>12.523999999999999</v>
+      </c>
+      <c r="G119">
+        <v>728.84900000000005</v>
+      </c>
+      <c r="H119">
+        <v>240.749</v>
+      </c>
+      <c r="I119">
+        <v>488.1</v>
+      </c>
+      <c r="J119">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K119">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>142.41999999999999</v>
+      </c>
+      <c r="B120">
+        <v>129.41800000000001</v>
+      </c>
+      <c r="C120">
+        <v>2.0720000000000001</v>
+      </c>
+      <c r="D120">
+        <v>142.41999999999999</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>12.539</v>
+      </c>
+      <c r="G120">
+        <v>727.27800000000002</v>
+      </c>
+      <c r="H120">
+        <v>240.31899999999999</v>
+      </c>
+      <c r="I120">
+        <v>486.959</v>
+      </c>
+      <c r="J120">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K120">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>151.46700000000001</v>
+      </c>
+      <c r="B121">
+        <v>128.81399999999999</v>
+      </c>
+      <c r="C121">
+        <v>2.0619999999999998</v>
+      </c>
+      <c r="D121">
+        <v>151.46700000000001</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>12.597</v>
+      </c>
+      <c r="G121">
+        <v>721.31500000000005</v>
+      </c>
+      <c r="H121">
+        <v>238.66300000000001</v>
+      </c>
+      <c r="I121">
+        <v>482.65199999999999</v>
+      </c>
+      <c r="J121">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K121">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>160.51499999999999</v>
+      </c>
+      <c r="B122">
+        <v>122.83</v>
+      </c>
+      <c r="C122">
+        <v>1.966</v>
+      </c>
+      <c r="D122">
+        <v>160.51499999999999</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>12.927</v>
+      </c>
+      <c r="G122">
+        <v>639.56600000000003</v>
+      </c>
+      <c r="H122">
+        <v>221.023</v>
+      </c>
+      <c r="I122">
+        <v>418.54199999999997</v>
+      </c>
+      <c r="J122">
+        <v>-1.2999999999999999E-2</v>
+      </c>
+      <c r="K122">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>169.56299999999999</v>
+      </c>
+      <c r="B123">
+        <v>89.742999999999995</v>
+      </c>
+      <c r="C123">
+        <v>1.4370000000000001</v>
+      </c>
+      <c r="D123">
+        <v>169.56299999999999</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <v>14.119</v>
+      </c>
+      <c r="G123">
+        <v>261.07900000000001</v>
+      </c>
+      <c r="H123">
+        <v>130.19800000000001</v>
+      </c>
+      <c r="I123">
+        <v>130.881</v>
+      </c>
+      <c r="J123">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="K123">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>178.61</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>178.61</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>24.974</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124">
+        <v>0</v>
+      </c>
+      <c r="J124">
+        <v>0</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>70</v>
+      </c>
+      <c r="B126">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>71</v>
+      </c>
+      <c r="B127">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>72</v>
+      </c>
+      <c r="B128">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>73</v>
+      </c>
+      <c r="B129">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>74</v>
+      </c>
+      <c r="B130">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>75</v>
+      </c>
+      <c r="B131">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>76</v>
+      </c>
+      <c r="B132">
+        <v>124907.628</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>77</v>
+      </c>
+      <c r="B133">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>28</v>
+      </c>
+      <c r="B134">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>78</v>
+      </c>
+      <c r="B135">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>79</v>
+      </c>
+      <c r="B136">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>80</v>
+      </c>
+      <c r="B137">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>32</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>81</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>82</v>
+      </c>
+      <c r="B140">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>83</v>
+      </c>
+      <c r="B141">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>84</v>
+      </c>
+      <c r="B142">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>85</v>
+      </c>
+      <c r="B143">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>86</v>
+      </c>
+      <c r="B144">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>87</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>88</v>
+      </c>
+      <c r="B146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>89</v>
+      </c>
+      <c r="B151" t="s">
+        <v>90</v>
+      </c>
+      <c r="C151" t="s">
+        <v>91</v>
+      </c>
+      <c r="D151" t="s">
+        <v>92</v>
+      </c>
+      <c r="E151" t="s">
+        <v>93</v>
+      </c>
+      <c r="F151" t="s">
+        <v>94</v>
+      </c>
+      <c r="G151" t="s">
+        <v>95</v>
+      </c>
+      <c r="H151" t="s">
+        <v>96</v>
+      </c>
+      <c r="I151" t="s">
+        <v>97</v>
+      </c>
+      <c r="J151" t="s">
+        <v>98</v>
+      </c>
+      <c r="K151" t="s">
+        <v>99</v>
+      </c>
+      <c r="L151" t="s">
+        <v>100</v>
+      </c>
+      <c r="M151" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>55</v>
+      </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>89</v>
+      </c>
+      <c r="B155" t="s">
+        <v>90</v>
+      </c>
+      <c r="C155" t="s">
+        <v>91</v>
+      </c>
+      <c r="D155" t="s">
+        <v>92</v>
+      </c>
+      <c r="E155" t="s">
+        <v>93</v>
+      </c>
+      <c r="F155" t="s">
+        <v>94</v>
+      </c>
+      <c r="G155" t="s">
+        <v>95</v>
+      </c>
+      <c r="H155" t="s">
+        <v>96</v>
+      </c>
+      <c r="I155" t="s">
+        <v>97</v>
+      </c>
+      <c r="J155" t="s">
+        <v>98</v>
+      </c>
+      <c r="K155" t="s">
+        <v>99</v>
+      </c>
+      <c r="L155" t="s">
+        <v>100</v>
+      </c>
+      <c r="M155" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>102</v>
+      </c>
+      <c r="B159" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2187DE66-CFC8-4538-BA60-F2792AEA8485}">
+  <dimension ref="A2:M159"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection sqref="A1:M159"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>39.968000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>24.984000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>178.43899999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>187.958</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>-8.9220000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>115.986</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>48.206000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>170.84200000000001</v>
+      </c>
+      <c r="C18">
+        <v>-9.9920000000000009</v>
+      </c>
+      <c r="D18">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>56693.084999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>180431.23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>79.319999999999993</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>4.0279999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>79.679000000000002</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>12.577</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24">
+        <v>0.99560000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25">
+        <v>0.94520000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>7231.134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28">
+        <v>79.638999999999996</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29">
+        <v>936333.58600000001</v>
+      </c>
+      <c r="C29" s="1">
+        <v>19826000</v>
+      </c>
+      <c r="D29" s="1">
+        <v>20762000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30">
+        <v>10315.251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36">
+        <v>140.61000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>-11.068</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>-2.117</v>
+      </c>
+      <c r="B45">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6.8330000000000002</v>
+      </c>
+      <c r="B46">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>15.784000000000001</v>
+      </c>
+      <c r="B47">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>24.734000000000002</v>
+      </c>
+      <c r="B48">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>33.683999999999997</v>
+      </c>
+      <c r="B49">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>42.634999999999998</v>
+      </c>
+      <c r="B50">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51.585000000000001</v>
+      </c>
+      <c r="B51">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>60.534999999999997</v>
+      </c>
+      <c r="B52">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>69.486000000000004</v>
+      </c>
+      <c r="B53">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>78.436000000000007</v>
+      </c>
+      <c r="B54">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>87.387</v>
+      </c>
+      <c r="B55">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>96.337000000000003</v>
+      </c>
+      <c r="B56">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>105.28700000000001</v>
+      </c>
+      <c r="B57">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>114.238</v>
+      </c>
+      <c r="B58">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>123.188</v>
+      </c>
+      <c r="B59">
+        <v>319.036</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>132.13800000000001</v>
+      </c>
+      <c r="B60">
+        <v>319.03399999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>141.089</v>
+      </c>
+      <c r="B61">
+        <v>318.91500000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>150.03899999999999</v>
+      </c>
+      <c r="B62">
+        <v>318.07799999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>158.99</v>
+      </c>
+      <c r="B63">
+        <v>304.20600000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>167.94</v>
+      </c>
+      <c r="B64">
+        <v>172.535</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>176.89</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>-11.39</v>
+      </c>
+      <c r="B69">
+        <v>576.31700000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>-2.3420000000000001</v>
+      </c>
+      <c r="B70">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>6.7050000000000001</v>
+      </c>
+      <c r="B71">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>15.753</v>
+      </c>
+      <c r="B72">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>24.800999999999998</v>
+      </c>
+      <c r="B73">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>33.847999999999999</v>
+      </c>
+      <c r="B74">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>42.896000000000001</v>
+      </c>
+      <c r="B75">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>51.944000000000003</v>
+      </c>
+      <c r="B76">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>60.991</v>
+      </c>
+      <c r="B77">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>70.039000000000001</v>
+      </c>
+      <c r="B78">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>79.085999999999999</v>
+      </c>
+      <c r="B79">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>88.134</v>
+      </c>
+      <c r="B80">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>97.182000000000002</v>
+      </c>
+      <c r="B81">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>106.229</v>
+      </c>
+      <c r="B82">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>115.277</v>
+      </c>
+      <c r="B83">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>124.325</v>
+      </c>
+      <c r="B84">
+        <v>998.49199999999996</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>133.37200000000001</v>
+      </c>
+      <c r="B85">
+        <v>998.48500000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>142.41999999999999</v>
+      </c>
+      <c r="B86">
+        <v>998.255</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>151.46700000000001</v>
+      </c>
+      <c r="B87">
+        <v>996.81399999999996</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>160.51499999999999</v>
+      </c>
+      <c r="B88">
+        <v>942.23599999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>169.56299999999999</v>
+      </c>
+      <c r="B89">
+        <v>553.51300000000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>178.61</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>55</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>56</v>
+      </c>
+      <c r="B93" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>58</v>
+      </c>
+      <c r="B96">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>55</v>
+      </c>
+      <c r="B97">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>59</v>
+      </c>
+      <c r="B98" t="s">
+        <v>60</v>
+      </c>
+      <c r="C98" t="s">
+        <v>61</v>
+      </c>
+      <c r="D98" t="s">
+        <v>62</v>
+      </c>
+      <c r="E98" t="s">
+        <v>63</v>
+      </c>
+      <c r="F98" t="s">
+        <v>64</v>
+      </c>
+      <c r="G98" t="s">
+        <v>65</v>
+      </c>
+      <c r="H98" t="s">
+        <v>66</v>
+      </c>
+      <c r="I98" t="s">
+        <v>67</v>
+      </c>
+      <c r="J98" t="s">
+        <v>68</v>
+      </c>
+      <c r="K98" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>-11.39</v>
+      </c>
+      <c r="B99">
+        <v>102.407</v>
+      </c>
+      <c r="C99">
+        <v>1.64</v>
+      </c>
+      <c r="D99">
+        <v>-11.39</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>17.713000000000001</v>
+      </c>
+      <c r="G99">
+        <v>374.00200000000001</v>
+      </c>
+      <c r="H99">
+        <v>78.775000000000006</v>
+      </c>
+      <c r="I99">
+        <v>295.22699999999998</v>
+      </c>
+      <c r="J99">
+        <v>9.157</v>
+      </c>
+      <c r="K99">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>-2.3420000000000001</v>
+      </c>
+      <c r="B100">
+        <v>129.56</v>
+      </c>
+      <c r="C100">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D100">
+        <v>-2.3420000000000001</v>
+      </c>
+      <c r="E100">
+        <v>1E-3</v>
+      </c>
+      <c r="F100">
+        <v>12.526</v>
+      </c>
+      <c r="G100">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H100">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I100">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J100">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K100">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>6.7050000000000001</v>
+      </c>
+      <c r="B101">
+        <v>129.56</v>
+      </c>
+      <c r="C101">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D101">
+        <v>6.7050000000000001</v>
+      </c>
+      <c r="E101">
+        <v>1E-3</v>
+      </c>
+      <c r="F101">
+        <v>12.526</v>
+      </c>
+      <c r="G101">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H101">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I101">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J101">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K101">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>15.753</v>
+      </c>
+      <c r="B102">
+        <v>129.56</v>
+      </c>
+      <c r="C102">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D102">
+        <v>15.753</v>
+      </c>
+      <c r="E102">
+        <v>1E-3</v>
+      </c>
+      <c r="F102">
+        <v>12.526</v>
+      </c>
+      <c r="G102">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H102">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I102">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J102">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K102">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>24.800999999999998</v>
+      </c>
+      <c r="B103">
+        <v>129.56</v>
+      </c>
+      <c r="C103">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D103">
+        <v>24.800999999999998</v>
+      </c>
+      <c r="E103">
+        <v>1E-3</v>
+      </c>
+      <c r="F103">
+        <v>12.526</v>
+      </c>
+      <c r="G103">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H103">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I103">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J103">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K103">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>33.847999999999999</v>
+      </c>
+      <c r="B104">
+        <v>129.56</v>
+      </c>
+      <c r="C104">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D104">
+        <v>33.847999999999999</v>
+      </c>
+      <c r="E104">
+        <v>1E-3</v>
+      </c>
+      <c r="F104">
+        <v>12.526</v>
+      </c>
+      <c r="G104">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H104">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I104">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J104">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K104">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>42.896000000000001</v>
+      </c>
+      <c r="B105">
+        <v>129.56</v>
+      </c>
+      <c r="C105">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D105">
+        <v>42.896000000000001</v>
+      </c>
+      <c r="E105">
+        <v>1E-3</v>
+      </c>
+      <c r="F105">
+        <v>12.526</v>
+      </c>
+      <c r="G105">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H105">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I105">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J105">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K105">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>51.944000000000003</v>
+      </c>
+      <c r="B106">
+        <v>129.56</v>
+      </c>
+      <c r="C106">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D106">
+        <v>51.944000000000003</v>
+      </c>
+      <c r="E106">
+        <v>1E-3</v>
+      </c>
+      <c r="F106">
+        <v>12.526</v>
+      </c>
+      <c r="G106">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H106">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I106">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J106">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K106">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>60.991</v>
+      </c>
+      <c r="B107">
+        <v>129.56</v>
+      </c>
+      <c r="C107">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D107">
+        <v>60.991</v>
+      </c>
+      <c r="E107">
+        <v>1E-3</v>
+      </c>
+      <c r="F107">
+        <v>12.526</v>
+      </c>
+      <c r="G107">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H107">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I107">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J107">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K107">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>70.039000000000001</v>
+      </c>
+      <c r="B108">
+        <v>129.56</v>
+      </c>
+      <c r="C108">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D108">
+        <v>70.039000000000001</v>
+      </c>
+      <c r="E108">
+        <v>1E-3</v>
+      </c>
+      <c r="F108">
+        <v>12.526</v>
+      </c>
+      <c r="G108">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H108">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I108">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J108">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K108">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>79.085999999999999</v>
+      </c>
+      <c r="B109">
+        <v>129.56</v>
+      </c>
+      <c r="C109">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D109">
+        <v>79.085999999999999</v>
+      </c>
+      <c r="E109">
+        <v>1E-3</v>
+      </c>
+      <c r="F109">
+        <v>12.526</v>
+      </c>
+      <c r="G109">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H109">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I109">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J109">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K109">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>88.134</v>
+      </c>
+      <c r="B110">
+        <v>129.56</v>
+      </c>
+      <c r="C110">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D110">
+        <v>88.134</v>
+      </c>
+      <c r="E110">
+        <v>1E-3</v>
+      </c>
+      <c r="F110">
+        <v>12.526</v>
+      </c>
+      <c r="G110">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H110">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I110">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J110">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K110">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>97.182000000000002</v>
+      </c>
+      <c r="B111">
+        <v>129.56</v>
+      </c>
+      <c r="C111">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D111">
+        <v>97.182000000000002</v>
+      </c>
+      <c r="E111">
+        <v>1E-3</v>
+      </c>
+      <c r="F111">
+        <v>12.526</v>
+      </c>
+      <c r="G111">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H111">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I111">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J111">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K111">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>106.229</v>
+      </c>
+      <c r="B112">
+        <v>129.56</v>
+      </c>
+      <c r="C112">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D112">
+        <v>106.229</v>
+      </c>
+      <c r="E112">
+        <v>1E-3</v>
+      </c>
+      <c r="F112">
+        <v>12.526</v>
+      </c>
+      <c r="G112">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H112">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I112">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J112">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K112">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>115.277</v>
+      </c>
+      <c r="B113">
+        <v>129.56</v>
+      </c>
+      <c r="C113">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D113">
+        <v>115.277</v>
+      </c>
+      <c r="E113">
+        <v>1E-3</v>
+      </c>
+      <c r="F113">
+        <v>12.526</v>
+      </c>
+      <c r="G113">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H113">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I113">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J113">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K113">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>124.325</v>
+      </c>
+      <c r="B114">
+        <v>129.56</v>
+      </c>
+      <c r="C114">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D114">
+        <v>124.325</v>
+      </c>
+      <c r="E114">
+        <v>1E-3</v>
+      </c>
+      <c r="F114">
+        <v>12.526</v>
+      </c>
+      <c r="G114">
+        <v>728.62699999999995</v>
+      </c>
+      <c r="H114">
+        <v>240.68899999999999</v>
+      </c>
+      <c r="I114">
+        <v>487.93900000000002</v>
+      </c>
+      <c r="J114">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K114">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>133.37200000000001</v>
+      </c>
+      <c r="B115">
+        <v>129.55600000000001</v>
+      </c>
+      <c r="C115">
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="D115">
+        <v>133.37200000000001</v>
+      </c>
+      <c r="E115">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F115">
+        <v>12.523999999999999</v>
+      </c>
+      <c r="G115">
+        <v>728.84900000000005</v>
+      </c>
+      <c r="H115">
+        <v>240.749</v>
+      </c>
+      <c r="I115">
+        <v>488.1</v>
+      </c>
+      <c r="J115">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K115">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>142.41999999999999</v>
+      </c>
+      <c r="B116">
+        <v>129.41800000000001</v>
+      </c>
+      <c r="C116">
+        <v>2.0720000000000001</v>
+      </c>
+      <c r="D116">
+        <v>142.41999999999999</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <v>12.539</v>
+      </c>
+      <c r="G116">
+        <v>727.27800000000002</v>
+      </c>
+      <c r="H116">
+        <v>240.31899999999999</v>
+      </c>
+      <c r="I116">
+        <v>486.959</v>
+      </c>
+      <c r="J116">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K116">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>151.46700000000001</v>
+      </c>
+      <c r="B117">
+        <v>128.81399999999999</v>
+      </c>
+      <c r="C117">
+        <v>2.0619999999999998</v>
+      </c>
+      <c r="D117">
+        <v>151.46700000000001</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117">
+        <v>12.597</v>
+      </c>
+      <c r="G117">
+        <v>721.31500000000005</v>
+      </c>
+      <c r="H117">
+        <v>238.66300000000001</v>
+      </c>
+      <c r="I117">
+        <v>482.65199999999999</v>
+      </c>
+      <c r="J117">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K117">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>160.51499999999999</v>
+      </c>
+      <c r="B118">
+        <v>122.83</v>
+      </c>
+      <c r="C118">
+        <v>1.966</v>
+      </c>
+      <c r="D118">
+        <v>160.51499999999999</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <v>12.927</v>
+      </c>
+      <c r="G118">
+        <v>639.56600000000003</v>
+      </c>
+      <c r="H118">
+        <v>221.023</v>
+      </c>
+      <c r="I118">
+        <v>418.54199999999997</v>
+      </c>
+      <c r="J118">
+        <v>-1.2999999999999999E-2</v>
+      </c>
+      <c r="K118">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>169.56299999999999</v>
+      </c>
+      <c r="B119">
+        <v>89.742999999999995</v>
+      </c>
+      <c r="C119">
+        <v>1.4370000000000001</v>
+      </c>
+      <c r="D119">
+        <v>169.56299999999999</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>14.119</v>
+      </c>
+      <c r="G119">
+        <v>261.07900000000001</v>
+      </c>
+      <c r="H119">
+        <v>130.19800000000001</v>
+      </c>
+      <c r="I119">
+        <v>130.881</v>
+      </c>
+      <c r="J119">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="K119">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>178.61</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>178.61</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>24.974</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120">
+        <v>0</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>70</v>
+      </c>
+      <c r="B122">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>71</v>
+      </c>
+      <c r="B123">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>72</v>
+      </c>
+      <c r="B124">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>73</v>
+      </c>
+      <c r="B125">
+        <v>7.984</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>74</v>
+      </c>
+      <c r="B126">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>75</v>
+      </c>
+      <c r="B127">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>76</v>
+      </c>
+      <c r="B128">
+        <v>124907.628</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>77</v>
+      </c>
+      <c r="B129">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>28</v>
+      </c>
+      <c r="B130">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>78</v>
+      </c>
+      <c r="B131">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>79</v>
+      </c>
+      <c r="B132">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>80</v>
+      </c>
+      <c r="B133">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>32</v>
+      </c>
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>81</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>82</v>
+      </c>
+      <c r="B136">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>83</v>
+      </c>
+      <c r="B137">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>84</v>
+      </c>
+      <c r="B138">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>85</v>
+      </c>
+      <c r="B139">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>86</v>
+      </c>
+      <c r="B140">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>87</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>88</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>89</v>
+      </c>
+      <c r="B147" t="s">
+        <v>90</v>
+      </c>
+      <c r="C147" t="s">
+        <v>91</v>
+      </c>
+      <c r="D147" t="s">
+        <v>92</v>
+      </c>
+      <c r="E147" t="s">
+        <v>93</v>
+      </c>
+      <c r="F147" t="s">
+        <v>94</v>
+      </c>
+      <c r="G147" t="s">
+        <v>95</v>
+      </c>
+      <c r="H147" t="s">
+        <v>96</v>
+      </c>
+      <c r="I147" t="s">
+        <v>97</v>
+      </c>
+      <c r="J147" t="s">
+        <v>98</v>
+      </c>
+      <c r="K147" t="s">
+        <v>99</v>
+      </c>
+      <c r="L147" t="s">
+        <v>100</v>
+      </c>
+      <c r="M147" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>55</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>89</v>
+      </c>
+      <c r="B151" t="s">
+        <v>90</v>
+      </c>
+      <c r="C151" t="s">
+        <v>91</v>
+      </c>
+      <c r="D151" t="s">
+        <v>92</v>
+      </c>
+      <c r="E151" t="s">
+        <v>93</v>
+      </c>
+      <c r="F151" t="s">
+        <v>94</v>
+      </c>
+      <c r="G151" t="s">
+        <v>95</v>
+      </c>
+      <c r="H151" t="s">
+        <v>96</v>
+      </c>
+      <c r="I151" t="s">
+        <v>97</v>
+      </c>
+      <c r="J151" t="s">
+        <v>98</v>
+      </c>
+      <c r="K151" t="s">
+        <v>99</v>
+      </c>
+      <c r="L151" t="s">
+        <v>100</v>
+      </c>
+      <c r="M151" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>102</v>
+      </c>
+      <c r="B155" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>